<commit_message>
Banco de dados parcialmente populado e burn up/down concluído
</commit_message>
<xml_diff>
--- a/Documentacao/graficoBurnUp&Down.xlsx
+++ b/Documentacao/graficoBurnUp&Down.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukki\Desktop\Facul\AutopecasMcQueen\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LukasReisdeOliveira\Desktop\Facul\AutopecasMcQueen\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7188CDE-20A8-4C15-B143-45C2346721A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1962BF5-58B3-48A1-94B7-9BE44C95B08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="59">
   <si>
     <t>SPRINT</t>
   </si>
@@ -227,18 +227,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -258,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -327,11 +321,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>Gráfico</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t> Burn Down</a:t>
+              <a:t>Gráfico Burn Down</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -375,7 +365,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.0535957998248447E-2"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.90087342019212269"/>
+          <c:h val="0.54380322251385238"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -384,7 +384,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burn Down'!$E$2</c:f>
+              <c:f>'Burn Down'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -470,51 +470,51 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Burn Down'!$E$3:$E$16</c:f>
+              <c:f>'Burn Down'!$D$3:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>243</c:v>
+                  <c:v>253</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>231</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>214</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>195</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>168</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>147</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>123</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>113</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>73</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-12</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,16 +522,16 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E545-4BCF-8403-B0BA1D5E00E0}"/>
+              <c16:uniqueId val="{00000008-352F-49DD-9F92-D8C917580E98}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burn Down'!$F$2</c:f>
+              <c:f>'Burn Down'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -543,9 +543,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -556,17 +554,12 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="dash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -578,37 +571,20 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="50000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="accent1"/>
                   </a:solidFill>
-                  <a:prstDash val="dash"/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="lgDash"/>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-E545-4BCF-8403-B0BA1D5E00E0}"/>
+                <c16:uniqueId val="{00000009-352F-49DD-9F92-D8C917580E98}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -619,37 +595,20 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
-                    <a:schemeClr val="accent6">
-                      <a:lumMod val="50000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="accent1"/>
                   </a:solidFill>
-                  <a:prstDash val="dash"/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="sysDash"/>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-E545-4BCF-8403-B0BA1D5E00E0}"/>
+                <c16:uniqueId val="{0000000A-352F-49DD-9F92-D8C917580E98}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -706,45 +665,45 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Burn Down'!$F$3:$F$16</c:f>
+              <c:f>'Burn Down'!$E$3:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>243</c:v>
+                  <c:v>253</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>226</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>207</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>180</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>159</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>135</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>125</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>85</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>10</c:v>
@@ -758,7 +717,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-E545-4BCF-8403-B0BA1D5E00E0}"/>
+              <c16:uniqueId val="{00000007-352F-49DD-9F92-D8C917580E98}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -777,7 +736,8 @@
         <c:axId val="294958392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="8"/>
+          <c:max val="15"/>
+          <c:min val="2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -835,11 +795,14 @@
         <c:crossAx val="294956792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="294956792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="300"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -897,6 +860,7 @@
         <c:crossAx val="294958392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="50"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1101,72 +1065,102 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Burn Up'!$A$3:$A$11</c:f>
+              <c:f>'Burn Up'!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Burn Up'!$B$3:$B$11</c:f>
+              <c:f>'Burn Up'!$B$3:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1500</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1500</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1500</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1500</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1700</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1700</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1700</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1700</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1700</c:v>
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1218,63 +1212,102 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Burn Up'!$A$3:$A$11</c:f>
+              <c:f>'Burn Up'!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Burn Up'!$E$3:$E$11</c:f>
+              <c:f>'Burn Up'!$E$3:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>550</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>750</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>750</c:v>
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1403,72 +1436,102 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'Burn Up'!$A$3:$A$11</c:f>
+              <c:f>'Burn Up'!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Burn Up'!$F$3:$F$11</c:f>
+              <c:f>'Burn Up'!$F$3:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>#N/A</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>#N/A</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>#N/A</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>#N/A</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1700</c:v>
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1495,6 +1558,8 @@
         <c:axId val="294958392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="15"/>
+          <c:min val="2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1552,6 +1617,7 @@
         <c:crossAx val="294956792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="294956792"/>
@@ -2808,22 +2874,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>144943</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>30557</xdr:rowOff>
+      <xdr:colOff>117232</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>139212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>562707</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>476251</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>106757</xdr:rowOff>
+      <xdr:rowOff>24912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA223DF-F65C-4DDC-BF48-116C386F66BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95506175-8B42-4F92-8B06-6BFC42AD95DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2852,13 +2918,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>47379</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>59989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>954236</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>136189</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3199,23 +3265,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60974E1B-3A99-44DF-886B-63181F317748}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -3235,7 +3302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3254,8 +3321,11 @@
       <c r="F2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -3274,8 +3344,11 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3295,7 +3368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3315,7 +3388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -3335,7 +3408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3355,7 +3428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -3375,7 +3448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -3395,7 +3468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -3415,7 +3488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -3435,7 +3508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -3455,12 +3528,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -3475,7 +3548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3495,7 +3568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -3515,7 +3588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -3535,7 +3608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3555,7 +3628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -3575,12 +3648,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -3595,12 +3668,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -3615,7 +3688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -3635,7 +3708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -3655,7 +3728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -3675,7 +3748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -3695,7 +3768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -3715,7 +3788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -3735,7 +3808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -3755,7 +3828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -3775,7 +3848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -3795,7 +3868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -3815,7 +3888,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3835,7 +3908,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -3855,7 +3928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -3875,7 +3948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -3895,7 +3968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -3915,7 +3988,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -3935,7 +4008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -3955,7 +4028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -3975,7 +4048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -3995,7 +4068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -4015,7 +4088,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -4035,7 +4108,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -4056,6 +4129,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Opção digitada não é válida!" error="Selecione uma opção da Lista" sqref="B2:B42" xr:uid="{C0DE89A6-C97F-40EA-8A72-333EB4DB2EE4}">
+      <formula1>$M$2:$M$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -4065,23 +4143,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B988CE95-B5BE-457A-8BE6-D647639C07CD}">
-  <dimension ref="A2:F17"/>
+  <dimension ref="A2:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4089,19 +4166,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4109,284 +4183,232 @@
         <v>265</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="E3">
-        <v>243</v>
-      </c>
-      <c r="F3">
-        <f>B4</f>
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>17</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <f>D3-C4</f>
+        <v>236</v>
       </c>
       <c r="E4">
-        <f>E3-D4</f>
-        <v>231</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F16" si="0">B5</f>
-        <v>226</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>17</v>
+        <f t="shared" ref="D5:D16" si="0">D4-C5</f>
+        <v>217</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E16" si="1">E4-D5</f>
-        <v>214</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="C6">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D6">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>198</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
-        <v>195</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="C7">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>27</v>
+        <f t="shared" si="0"/>
+        <v>183</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
-        <v>168</v>
-      </c>
-      <c r="F7">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>169</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>159</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>159</v>
-      </c>
-      <c r="C8">
-        <v>24</v>
-      </c>
-      <c r="D8">
-        <v>21</v>
-      </c>
       <c r="E8">
-        <f t="shared" si="1"/>
-        <v>147</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>145</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="E9">
         <v>135</v>
       </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>24</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>123</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C10">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
-        <v>81</v>
-      </c>
-      <c r="F11">
-        <f>B12</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C12">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C13">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>31</v>
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C14">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C15">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4394,28 +4416,20 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>146</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
-        <v>-12</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17">
-        <f>SUM(C3:C11)</f>
-        <v>522</v>
-      </c>
-      <c r="D17">
-        <f>SUM(D4:D16)</f>
-        <v>255</v>
+        <f>SUM(C4:C16)</f>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4426,22 +4440,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34115AC9-461F-43DA-980F-2B17E5628FD0}">
-  <dimension ref="A2:F12"/>
+  <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F2" sqref="A2:F2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4461,198 +4475,310 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>1500</v>
+        <v>265</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <f>D3</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>1500</v>
+        <v>265</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2">
-        <v>200</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <f>E3+D4</f>
-        <v>200</v>
-      </c>
-      <c r="F4" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>1500</v>
+        <v>265</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <f>E4+D5</f>
-        <v>300</v>
-      </c>
-      <c r="F5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="F5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>1500</v>
+        <v>265</v>
       </c>
       <c r="C6">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="D6" s="2">
-        <v>250</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <f>E5+D6</f>
-        <v>550</v>
-      </c>
-      <c r="F6" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="F6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>1700</v>
+        <v>265</v>
       </c>
       <c r="C7">
-        <v>200</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2">
-        <v>200</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <f>E6+D7</f>
-        <v>750</v>
-      </c>
-      <c r="F7" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="F7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>1700</v>
+        <v>265</v>
       </c>
       <c r="C8">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="D8" s="2">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E8">
         <f>E7+D8</f>
-        <v>750</v>
-      </c>
-      <c r="F8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="F8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>1700</v>
+        <v>265</v>
       </c>
       <c r="C9">
-        <v>220</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="F9" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E16" si="0">E8+D9</f>
+        <v>109</v>
+      </c>
+      <c r="F9">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>1700</v>
+        <v>265</v>
       </c>
       <c r="C10">
-        <v>230</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="F10" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+      <c r="D10" s="2">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="F10">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>1700</v>
+        <v>265</v>
       </c>
       <c r="C11">
-        <v>230</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>170</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
       <c r="F11">
-        <f>B11</f>
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>265</v>
+      </c>
       <c r="C12">
-        <f>SUM(C3:C11)</f>
-        <v>1700</v>
-      </c>
-      <c r="D12">
-        <f>SUM(D3:D11)</f>
-        <v>750</v>
+        <v>201</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="F12">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>265</v>
+      </c>
+      <c r="C13">
+        <v>218</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="F13">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>265</v>
+      </c>
+      <c r="C14">
+        <v>237</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="F14">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>265</v>
+      </c>
+      <c r="C15">
+        <v>255</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="F15">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>265</v>
+      </c>
+      <c r="C16">
+        <v>265</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="F16">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>SUM(D3:D16)</f>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Cadastro de cliente construído
</commit_message>
<xml_diff>
--- a/Documentacao/graficoBurnUp&Down.xlsx
+++ b/Documentacao/graficoBurnUp&Down.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LukasReisdeOliveira\Desktop\Facul\AutopecasMcQueen\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1962BF5-58B3-48A1-94B7-9BE44C95B08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B38889-BBDB-4889-B37B-6AA05E933B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
   </bookViews>
@@ -218,8 +218,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -247,12 +255,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2955,7 +2964,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11FCB6D5-9697-46D7-B7A7-A210CF4510F3}" name="Product_Backlog" displayName="Product_Backlog" ref="A1:F42" totalsRowShown="0">
-  <autoFilter ref="A1:F42" xr:uid="{11FCB6D5-9697-46D7-B7A7-A210CF4510F3}"/>
+  <autoFilter ref="A1:F42" xr:uid="{11FCB6D5-9697-46D7-B7A7-A210CF4510F3}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Em Aberto"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A8CF0624-9547-42BA-8CE5-855447108A79}" name="Item" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{27872076-ACB9-4388-BF47-24E91B27C8C6}" name="Status" dataDxfId="3"/>
@@ -3267,8 +3282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60974E1B-3A99-44DF-886B-63181F317748}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3302,7 +3317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3325,7 +3340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -3348,7 +3363,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3368,7 +3383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3388,7 +3403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -3408,7 +3423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3428,7 +3443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -3448,7 +3463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -3468,7 +3483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -3488,7 +3503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -3508,7 +3523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -3548,7 +3563,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -3568,7 +3583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -3588,7 +3603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -3608,7 +3623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3628,7 +3643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -3648,7 +3663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -3668,7 +3683,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -3688,7 +3703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -3832,7 +3847,7 @@
       <c r="A28" t="s">
         <v>45</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C28" t="s">
@@ -4135,8 +4150,9 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Atualização do backlog e casos de teste concluidos
</commit_message>
<xml_diff>
--- a/Documentacao/graficoBurnUp&Down.xlsx
+++ b/Documentacao/graficoBurnUp&Down.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LukasReisdeOliveira\Desktop\Facul\AutopecasMcQueen\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B38889-BBDB-4889-B37B-6AA05E933B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1617B3-790D-49FB-A0BC-0CBADEFF1722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="4" r:id="rId1"/>
@@ -218,16 +218,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -261,7 +253,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,25 +497,25 @@
                   <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>146</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>146</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>146</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>146</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>146</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>146</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>146</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1298,25 +1290,25 @@
                   <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>119</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>119</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>119</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>119</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>119</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>119</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>119</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3282,8 +3274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60974E1B-3A99-44DF-886B-63181F317748}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3723,12 +3715,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
@@ -4162,7 +4154,7 @@
   <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4324,11 +4316,11 @@
         <v>135</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E10">
         <v>103</v>
@@ -4345,8 +4337,8 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>146</v>
+        <f>D10-C11</f>
+        <v>139</v>
       </c>
       <c r="E11">
         <v>95</v>
@@ -4364,7 +4356,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E12">
         <v>64</v>
@@ -4382,7 +4374,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E13">
         <v>47</v>
@@ -4400,7 +4392,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E14">
         <v>28</v>
@@ -4418,7 +4410,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -4436,7 +4428,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4445,7 +4437,7 @@
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17">
         <f>SUM(C4:C16)</f>
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -4458,8 +4450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34115AC9-461F-43DA-980F-2B17E5628FD0}">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4649,11 +4641,11 @@
         <v>162</v>
       </c>
       <c r="D10" s="2">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F10">
         <v>162</v>
@@ -4674,7 +4666,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F11">
         <v>170</v>
@@ -4695,7 +4687,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F12">
         <v>201</v>
@@ -4716,7 +4708,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F13">
         <v>218</v>
@@ -4737,7 +4729,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F14">
         <v>237</v>
@@ -4758,7 +4750,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F15">
         <v>255</v>
@@ -4779,7 +4771,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F16">
         <v>265</v>
@@ -4788,7 +4780,7 @@
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D16)</f>
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção da rota de exclusão de fornecedor e finalização do grid de novas vendas
</commit_message>
<xml_diff>
--- a/Documentacao/graficoBurnUp&Down.xlsx
+++ b/Documentacao/graficoBurnUp&Down.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LukasReisdeOliveira\Desktop\Facul\AutopecasMcQueen\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A56AC3-A7CE-4D3C-B28A-1D32B178A427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F241CBE-F945-4CE8-95F6-92FBB5653879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
+    <workbookView xWindow="20370" yWindow="-2400" windowWidth="29040" windowHeight="15720" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="4" r:id="rId1"/>
@@ -503,19 +503,19 @@
                   <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>115</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>115</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>115</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>115</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>115</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1296,19 +1296,19 @@
                   <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>150</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>150</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>150</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>150</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>150</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3274,8 +3274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60974E1B-3A99-44DF-886B-63181F317748}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3855,12 +3855,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
         <v>25</v>
@@ -4153,8 +4153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B988CE95-B5BE-457A-8BE6-D647639C07CD}">
   <dimension ref="A2:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4352,11 +4352,11 @@
         <v>95</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E12">
         <v>64</v>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E13">
         <v>47</v>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E14">
         <v>28</v>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4437,7 +4437,7 @@
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17">
         <f>SUM(C4:C16)</f>
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -4451,7 +4451,7 @@
   <dimension ref="A2:F17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4683,11 +4683,11 @@
         <v>201</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F12">
         <v>201</v>
@@ -4708,7 +4708,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F13">
         <v>218</v>
@@ -4729,7 +4729,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F14">
         <v>237</v>
@@ -4750,7 +4750,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F15">
         <v>255</v>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="F16">
         <v>265</v>
@@ -4780,7 +4780,7 @@
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>SUM(D3:D16)</f>
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>